<commit_message>
volunteer upload done, events attendance done
</commit_message>
<xml_diff>
--- a/uploads/School_membership_database.xlsx
+++ b/uploads/School_membership_database.xlsx
@@ -1,29 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24102"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/megwu/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://lincolnuniac-my.sharepoint.com/personal/jack_swannell_childrensuniversity_co_nz/Documents/Admin/IT/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{F5AC746E-0D63-4E3B-BFC1-4516A0E9AC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D038AF6-EBCA-478C-BF67-DD4A910AD287}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{9760B367-9F6D-4E18-A6B4-220D24FD9DAF}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 active list" sheetId="1" r:id="rId1"/>
     <sheet name="Waiting list" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -40,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -60,12 +55,39 @@
     <t>Status</t>
   </si>
   <si>
+    <t>2019 Total</t>
+  </si>
+  <si>
+    <t>Returning #</t>
+  </si>
+  <si>
+    <t>2020 Total</t>
+  </si>
+  <si>
+    <t>Max # 2021</t>
+  </si>
+  <si>
+    <t>Requested/ confirmed #</t>
+  </si>
+  <si>
+    <t>Coordinator</t>
+  </si>
+  <si>
     <t>Training</t>
   </si>
   <si>
     <t>Launch</t>
   </si>
   <si>
+    <t>Passport presentation</t>
+  </si>
+  <si>
+    <t>Portal / Passports</t>
+  </si>
+  <si>
+    <t>Agreement/ consent</t>
+  </si>
+  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -90,6 +112,9 @@
     <t>NA</t>
   </si>
   <si>
+    <t>Y/Y</t>
+  </si>
+  <si>
     <t>Agreement signed, consent form recieved</t>
   </si>
   <si>
@@ -148,78 +173,24 @@
   </si>
   <si>
     <t>Decile 5, CCC</t>
-  </si>
-  <si>
-    <t>School ID</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Year</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Returning Number</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Total</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Max Number2021</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Confirmed Number</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Coordinator ID</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Passport Presentation</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Portal</t>
-  </si>
-  <si>
-    <t>Passports</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Agreement</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Consent</t>
-    <phoneticPr fontId="8" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -227,7 +198,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -235,7 +206,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -243,7 +214,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -251,25 +222,19 @@
       <b/>
       <sz val="20"/>
       <color theme="0"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -322,7 +287,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -366,14 +331,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="2" builtinId="8"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -684,37 +646,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245A3F59-27F0-41BF-BD9C-9387E8B76DD9}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T9"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="6" width="10" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" customWidth="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1"/>
-    <col min="12" max="12" width="19.5" customWidth="1"/>
-    <col min="14" max="14" width="12.5" customWidth="1"/>
-    <col min="15" max="16" width="22" customWidth="1"/>
-    <col min="17" max="18" width="17.33203125" customWidth="1"/>
-    <col min="19" max="19" width="21.1640625" customWidth="1"/>
-    <col min="20" max="20" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="19.42578125" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="22" customWidth="1"/>
+    <col min="16" max="16" width="17.28515625" customWidth="1"/>
+    <col min="17" max="17" width="21.140625" customWidth="1"/>
+    <col min="18" max="18" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -731,76 +693,70 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>37</v>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4">
-        <v>2019</v>
+        <v>22</v>
+      </c>
+      <c r="G2" s="5">
+        <v>19</v>
       </c>
       <c r="H2" s="5">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="I2" s="5">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="J2" s="5">
         <v>40</v>
@@ -809,58 +765,54 @@
         <v>25</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="O2" s="7">
         <v>44270</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>16</v>
+        <v>25</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" s="3"/>
-      <c r="H3" s="5">
+        <v>30</v>
+      </c>
+      <c r="G3" s="5">
         <v>0</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>15</v>
+      <c r="H3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="5">
+        <v>25</v>
       </c>
       <c r="J3" s="5">
         <v>30</v>
@@ -869,7 +821,7 @@
         <v>39</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="M3" s="7">
         <v>44242</v>
@@ -880,56 +832,48 @@
       <c r="O3" s="7">
         <v>44278</v>
       </c>
-      <c r="P3" s="7" t="s">
-        <v>48</v>
+      <c r="P3" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="R3" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18">
       <c r="F9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" s="15"/>
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77DE09CD-CAAF-4B79-A580-AAAD0B124CC0}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.83203125" customWidth="1"/>
-    <col min="5" max="5" width="26.5" customWidth="1"/>
-    <col min="6" max="6" width="25.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="26.25">
       <c r="A1" s="8" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -937,80 +881,80 @@
       <c r="E1" s="8"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" s="9">
         <v>1</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="9">
         <v>2</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G4" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{B0341571-C30F-4A6A-A58B-18EE0CBF3098}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100840061F9DC321B428F6D5C5DB03A1A63" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4ef34e0891b7e78f128c981ac5712e9f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180eb382-7469-4407-b6a7-9e3c553560d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="017260f72885d0d62c8e4e105bf0de37" ns2:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100840061F9DC321B428F6D5C5DB03A1A63" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="218d44522063d3e139a84098689cd5f5">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="180eb382-7469-4407-b6a7-9e3c553560d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7bb75e2003902cea2fab401753615262" ns2:_="">
     <xsd:import namespace="180eb382-7469-4407-b6a7-9e3c553560d8"/>
     <xsd:element name="properties">
       <xsd:complexType>
@@ -1027,7 +971,6 @@
                 <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1085,11 +1028,6 @@
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
         </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="17" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -1208,36 +1146,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E7C40C1-CDA0-4423-9B4A-14213697C7E6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="180eb382-7469-4407-b6a7-9e3c553560d8"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D43D9ECA-BC92-4EB7-AF29-904B9AB11EFF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3A7E450-2743-4924-88D9-8F14A40D3281}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C3A7E450-2743-4924-88D9-8F14A40D3281}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284EDF83-74B2-4946-82CB-E59A3109F313}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{284EDF83-74B2-4946-82CB-E59A3109F313}"/>
 </file>
</xml_diff>